<commit_message>
support for Windows GUI autotest
</commit_message>
<xml_diff>
--- a/sweetest/testcase/Echo-TestCase.xlsx
+++ b/sweetest/testcase/Echo-TestCase.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="105" windowWidth="25785" windowHeight="12210"/>
+    <workbookView xWindow="270" yWindow="105" windowWidth="25785" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="echo" sheetId="9" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <definedName name="雪球行情中心">#REF!</definedName>
     <definedName name="页面">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>测试数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,13 +160,57 @@
   <si>
     <t>status_code=200,
 json={'args': {'foo1': 'bar1'\,'foo2': 'bar2'}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NotePad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帮助(H)-&gt;关于记事本(A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于"记事本"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLICK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INPUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无标题 - 记事本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无标题 - 记事本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello world!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="177" formatCode="0_ ;[Red]\-0\ "/>
@@ -303,6 +347,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -350,7 +397,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,7 +432,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,7 +646,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -608,10 +655,10 @@
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="11.875" customWidth="1"/>
     <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
-    <col min="6" max="6" width="8.625" customWidth="1"/>
-    <col min="7" max="7" width="20.625" customWidth="1"/>
-    <col min="8" max="8" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
+    <col min="8" max="8" width="66.5" customWidth="1"/>
     <col min="9" max="9" width="48.5" customWidth="1"/>
     <col min="10" max="10" width="33.125" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
@@ -803,12 +850,22 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -823,10 +880,18 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -841,11 +906,21 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1362,7 +1437,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" sqref="E4:E1048576 E1"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" sqref="E1 E4:E1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" sqref="G2:G3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>